<commit_message>
refactor data-manipulation and shape-data
</commit_message>
<xml_diff>
--- a/data/testdata/test_file_xlsx_col.xlsx
+++ b/data/testdata/test_file_xlsx_col.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -175,28 +175,31 @@
     <t xml:space="preserve">Datumsangaben</t>
   </si>
   <si>
+    <t xml:space="preserve">1.1 – 2. Dez. 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. - 2. Dez. 1900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. August 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17. 08. 0050</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2.023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Fevrier 1823</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 Agosto 172</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.1.2012</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Dez. 1900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. August 2001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17. 08. 0050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.2.023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Février 1823</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 Agosto 172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Février 200</t>
+    <t xml:space="preserve">2 Fevrier 200</t>
   </si>
 </sst>
 </file>
@@ -207,11 +210,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -230,15 +234,10 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -283,8 +282,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -292,19 +299,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -327,8 +322,8 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,230 +332,230 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="I7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="3" t="s">
-        <v>51</v>
+      <c r="J7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
refactor small stuff and update readme
</commit_message>
<xml_diff>
--- a/data/testdata/test_file_xlsx_col.xlsx
+++ b/data/testdata/test_file_xlsx_col.xlsx
@@ -322,8 +322,8 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -481,11 +481,26 @@
       <c r="D5" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="E5" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <v>6</v>
+      </c>
       <c r="H5" s="1" t="s">
         <v>47</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>